<commit_message>
criando interface grafica para enviar arquivo e gerar o relatorio separado
</commit_message>
<xml_diff>
--- a/relatorios_simplificados/separarNeomater_SIMPLIFICADO.xlsx
+++ b/relatorios_simplificados/separarNeomater_SIMPLIFICADO.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Por Município Colunas" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Por Municipio Colunas" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Dados Detalhados" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
@@ -2106,7 +2106,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Município</t>
+          <t>Municipio</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -2146,7 +2146,7 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Sedação</t>
+          <t>Sedacao</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">

</xml_diff>